<commit_message>
done for first 100
</commit_message>
<xml_diff>
--- a/first200.xlsx
+++ b/first200.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leslieren/Desktop/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F615109-F072-5548-A529-CB7D976B8665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A5E30E-F9DD-AF4A-9B4C-EB0E57A3BCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15240" xr2:uid="{FE1163BA-F853-5542-82D9-7552C7288314}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="264">
   <si>
     <t>Two Sum</t>
   </si>
@@ -604,6 +604,228 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/climbing-stairs/</t>
+  </si>
+  <si>
+    <t>Simplify Path</t>
+  </si>
+  <si>
+    <t>stack-pq</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/simplify-path/</t>
+  </si>
+  <si>
+    <t>Edit Distance</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/edit-distance/</t>
+  </si>
+  <si>
+    <t>Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/set-matrix-zeroes/</t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-a-2d-matrix/</t>
+  </si>
+  <si>
+    <t>Sort Colors</t>
+  </si>
+  <si>
+    <t>one pass not yet</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-colors/</t>
+  </si>
+  <si>
+    <t>Minimum Window Substring</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-window-substring/</t>
+  </si>
+  <si>
+    <t>Combinations</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combinations/</t>
+  </si>
+  <si>
+    <t>great problem, transition between iterative and recursive</t>
+  </si>
+  <si>
+    <t>Subsets</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subsets/</t>
+  </si>
+  <si>
+    <t>Word Search</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-duplicates-from-sorted-array-ii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-search/</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-in-rotated-sorted-array-ii/</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted List II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-duplicates-from-sorted-list/</t>
+  </si>
+  <si>
+    <t>Largest Rectangle in Histogram</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/largest-rectangle-in-histogram/</t>
+  </si>
+  <si>
+    <t>one edge case emitted</t>
+  </si>
+  <si>
+    <t>Maximal Rectangle</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximal-rectangle/</t>
+  </si>
+  <si>
+    <t>cannot understand the dp solution</t>
+  </si>
+  <si>
+    <t>Partition List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/partition-list/submissions/</t>
+  </si>
+  <si>
+    <t>Scramble String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/scramble-string/</t>
+  </si>
+  <si>
+    <t>dp not yet</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>O(m+n)! 想了好一会儿才想出来</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-sorted-array/</t>
+  </si>
+  <si>
+    <t>Gray Code</t>
+  </si>
+  <si>
+    <t>Subsets II</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/gray-code/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subsets-ii/</t>
+  </si>
+  <si>
+    <t>iterative not yet, in essence, this is the same as problem40</t>
+  </si>
+  <si>
+    <t>Decode Ways</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/decode-ways/submissions/</t>
+  </si>
+  <si>
+    <t>别人的思路简单一点点</t>
+  </si>
+  <si>
+    <t>Reverse Linked List II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list-ii/</t>
+  </si>
+  <si>
+    <t>Restore IP Addresses</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/restore-ip-addresses/</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>Binary Tree Inorder Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-inorder-traversal/</t>
+  </si>
+  <si>
+    <t>Unique Binary Search Trees II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-binary-search-trees-ii/</t>
+  </si>
+  <si>
+    <t>dp not yet, 可以先想想下一道dp咋做</t>
+  </si>
+  <si>
+    <t>Unique Binary Search Trees</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-binary-search-trees/</t>
+  </si>
+  <si>
+    <t>Interleaving String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/interleaving-string/</t>
+  </si>
+  <si>
+    <t>be careful in dp</t>
+  </si>
+  <si>
+    <t>Validate Binary Search Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/validate-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>Recover Binary Search Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/recover-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>可以再做做，稍微想了一下</t>
+  </si>
+  <si>
+    <t>Same Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/same-tree/</t>
   </si>
 </sst>
 </file>
@@ -1028,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF1DFDB-3B0E-374C-823F-F15857147895}">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="158" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:B75"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="158" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2216,6 +2438,497 @@
       </c>
       <c r="I75" s="2" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="4">
+        <v>44348</v>
+      </c>
+      <c r="B76">
+        <v>71</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>72</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>73</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>74</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>75</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="4">
+        <v>44349</v>
+      </c>
+      <c r="B81">
+        <v>76</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>77</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>78</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>79</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>80</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="4">
+        <v>44350</v>
+      </c>
+      <c r="B86">
+        <v>81</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>82</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>83</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>84</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>85</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="4">
+        <v>44351</v>
+      </c>
+      <c r="B91">
+        <v>86</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>87</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>88</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>89</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>90</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="4">
+        <v>44352</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="4">
+        <v>44353</v>
+      </c>
+      <c r="B97">
+        <v>91</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B98">
+        <v>92</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B99">
+        <v>93</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>94</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>95</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>96</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B103">
+        <v>97</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>98</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" s="4">
+        <v>44354</v>
+      </c>
+      <c r="B105">
+        <v>99</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>100</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2293,6 +3006,36 @@
     <hyperlink ref="I73" r:id="rId71" xr:uid="{630962D8-A7D6-F14C-9040-858093294E4F}"/>
     <hyperlink ref="I74" r:id="rId72" xr:uid="{71AAC5CD-983B-394C-A4BC-77FBAF4CC1DB}"/>
     <hyperlink ref="I75" r:id="rId73" xr:uid="{8C7239F7-3AD2-DD4C-B294-CC16C247073A}"/>
+    <hyperlink ref="I76" r:id="rId74" xr:uid="{88040107-B423-A249-87CE-380AFA293C53}"/>
+    <hyperlink ref="I77" r:id="rId75" xr:uid="{74C12C3D-5CD8-DD4B-B622-BE91DBD0B9D3}"/>
+    <hyperlink ref="I78" r:id="rId76" xr:uid="{50C53A9C-C904-CD48-BD3D-1383DB315EE7}"/>
+    <hyperlink ref="I79" r:id="rId77" xr:uid="{EF7F5D61-F812-B64E-9D84-CDAF92072EA7}"/>
+    <hyperlink ref="I80" r:id="rId78" xr:uid="{8DCE80DA-D0F7-3D40-B0E1-5D6C7E2B969D}"/>
+    <hyperlink ref="I81" r:id="rId79" xr:uid="{DC9A893B-7D7B-F24C-9B86-34AF430168DE}"/>
+    <hyperlink ref="I82" r:id="rId80" xr:uid="{73BCABE9-55B6-1849-AB22-4657F0258362}"/>
+    <hyperlink ref="I83" r:id="rId81" xr:uid="{4B7A4072-CAAA-2348-8FCB-9A8F847A1BA6}"/>
+    <hyperlink ref="I85" r:id="rId82" xr:uid="{961329D8-EFD4-CD49-B20D-FC915A755238}"/>
+    <hyperlink ref="I84" r:id="rId83" xr:uid="{68982647-04E5-FD41-9A3F-5406BB8CC131}"/>
+    <hyperlink ref="I86" r:id="rId84" xr:uid="{FE0EF311-436B-BD48-8889-5A9E43D914A6}"/>
+    <hyperlink ref="I87" r:id="rId85" xr:uid="{0E8CB090-1EE4-3140-B1FC-DA519403B837}"/>
+    <hyperlink ref="I88" r:id="rId86" xr:uid="{3756E286-D8F7-2648-B123-1A2A321D8293}"/>
+    <hyperlink ref="I89" r:id="rId87" xr:uid="{04764BDC-9D3F-4141-B1D1-18580FFE9926}"/>
+    <hyperlink ref="I90" r:id="rId88" xr:uid="{38A17CFF-0464-D143-9FE2-CFC443E75245}"/>
+    <hyperlink ref="I91" r:id="rId89" xr:uid="{84B43AC2-41FA-044F-80D3-A127AEE8F639}"/>
+    <hyperlink ref="I92" r:id="rId90" xr:uid="{B7275D8C-A315-864B-A728-4CB700D6AC8E}"/>
+    <hyperlink ref="I93" r:id="rId91" xr:uid="{777DED19-61F4-F34B-92A6-FC3785E696F5}"/>
+    <hyperlink ref="I94" r:id="rId92" xr:uid="{4034314E-8B98-6A43-80B0-B94CA2A47837}"/>
+    <hyperlink ref="I95" r:id="rId93" xr:uid="{D0521A48-CB4A-524D-953D-50BABF6A9ED2}"/>
+    <hyperlink ref="I97" r:id="rId94" xr:uid="{34D801E1-DF0C-7C44-AA7E-55282D9DC2AE}"/>
+    <hyperlink ref="I98" r:id="rId95" xr:uid="{4AA53E0D-6B85-8B40-9E89-8709B0A807E0}"/>
+    <hyperlink ref="I99" r:id="rId96" xr:uid="{2766E828-B1D3-DB4B-93FA-16406B7D8D57}"/>
+    <hyperlink ref="I100" r:id="rId97" xr:uid="{BDD3104F-059B-214F-89E1-23EB71A28504}"/>
+    <hyperlink ref="I101" r:id="rId98" xr:uid="{E7C4B93F-6890-E446-B18B-58195C71EC08}"/>
+    <hyperlink ref="I102" r:id="rId99" xr:uid="{F75D22B4-05B6-8946-91F5-247984FC50F1}"/>
+    <hyperlink ref="I103" r:id="rId100" xr:uid="{82525C4C-C443-2441-B86B-A49A757E2FC4}"/>
+    <hyperlink ref="I104" r:id="rId101" xr:uid="{A39FF3BB-7F7F-CC48-AEFC-34269EEADB06}"/>
+    <hyperlink ref="I105" r:id="rId102" xr:uid="{D2C587ED-991A-F240-A45D-61AF67D9BA87}"/>
+    <hyperlink ref="I106" r:id="rId103" xr:uid="{628B66FB-BE95-3E48-B2D8-A20797DF7D0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
done for first 200
</commit_message>
<xml_diff>
--- a/first200.xlsx
+++ b/first200.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leslieren/Desktop/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A5E30E-F9DD-AF4A-9B4C-EB0E57A3BCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8E75C2-7643-5041-8184-FCCBEBF3ADC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15240" xr2:uid="{FE1163BA-F853-5542-82D9-7552C7288314}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{FE1163BA-F853-5542-82D9-7552C7288314}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="475">
   <si>
     <t>Two Sum</t>
   </si>
@@ -826,6 +826,639 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/same-tree/</t>
+  </si>
+  <si>
+    <t>Symmetric Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/symmetric-tree/</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-level-order-traversal/</t>
+  </si>
+  <si>
+    <t>Binary Tree Zigzag Level Order Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-zigzag-level-order-traversal/</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-depth-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>Construct Binary Tree from Preorder and Inorder Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/</t>
+  </si>
+  <si>
+    <t>可以再做，optimize</t>
+  </si>
+  <si>
+    <t>Construct Binary Tree from Inorder and Postorder Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/construct-binary-tree-from-inorder-and-postorder-traversal/</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-level-order-traversal-ii/</t>
+  </si>
+  <si>
+    <t>Convert Sorted Array to Binary Search Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/convert-sorted-array-to-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>Just try the iterative one</t>
+  </si>
+  <si>
+    <t>Convert Sorted List to Binary Search Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/convert-sorted-list-to-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/balanced-binary-tree/</t>
+  </si>
+  <si>
+    <t>Minimum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-depth-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>Path Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum/</t>
+  </si>
+  <si>
+    <t>didn't think thoroughly</t>
+  </si>
+  <si>
+    <t>Path Sum II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum-ii/</t>
+  </si>
+  <si>
+    <t>Flatten Binary Tree to Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/flatten-binary-tree-to-linked-list/</t>
+  </si>
+  <si>
+    <t>$ 可以再看看解法</t>
+  </si>
+  <si>
+    <t>$ Solution3 is kind of like the one in 106</t>
+  </si>
+  <si>
+    <t>$$ kind like 109&amp;106</t>
+  </si>
+  <si>
+    <t>Distinct Subsequences</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/distinct-subsequences/</t>
+  </si>
+  <si>
+    <t>dp要想一下才能做出来</t>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/populating-next-right-pointers-in-each-node/</t>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node II</t>
+  </si>
+  <si>
+    <t>$$</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/populating-next-right-pointers-in-each-node-ii/</t>
+  </si>
+  <si>
+    <t>Pascal's Triangle</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/pascals-triangle/</t>
+  </si>
+  <si>
+    <t>Pascal's Triangle II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/pascals-triangle-ii/</t>
+  </si>
+  <si>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/triangle/</t>
+  </si>
+  <si>
+    <t>c comment</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-ii/</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock III</t>
+  </si>
+  <si>
+    <t>$$not yet</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-iii/</t>
+  </si>
+  <si>
+    <t>Binary Tree Maximum Path Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-maximum-path-sum/</t>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-palindrome/</t>
+  </si>
+  <si>
+    <t>Word Ladder II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-ladder-ii/</t>
+  </si>
+  <si>
+    <t>Word Ladder</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-ladder/</t>
+  </si>
+  <si>
+    <t>Sum Root to Leaf Numbers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sum-root-to-leaf-numbers/</t>
+  </si>
+  <si>
+    <t>Longest Consecutive Sequence</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-consecutive-sequence/</t>
+  </si>
+  <si>
+    <t>Surrounded Regions</t>
+  </si>
+  <si>
+    <t>可以先从不合格的开始思考</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/surrounded-regions/</t>
+  </si>
+  <si>
+    <t>Palindrome Partitioning</t>
+  </si>
+  <si>
+    <t>try divide and conquer</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-partitioning/submissions/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-partitioning-ii/</t>
+  </si>
+  <si>
+    <t>Palindrome Partitioning II</t>
+  </si>
+  <si>
+    <t>Clone Graph</t>
+  </si>
+  <si>
+    <t>graph</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/clone-graph/</t>
+  </si>
+  <si>
+    <t>Gas Station</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/gas-station/</t>
+  </si>
+  <si>
+    <t>Single Number</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/single-number/</t>
+  </si>
+  <si>
+    <t>not yet$$$</t>
+  </si>
+  <si>
+    <t>Candy</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/candy/</t>
+  </si>
+  <si>
+    <t>Single Number II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/single-number-ii/</t>
+  </si>
+  <si>
+    <t>Copy List with Random Pointer</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/copy-list-with-random-pointer/</t>
+  </si>
+  <si>
+    <t>Word Break</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-break/</t>
+  </si>
+  <si>
+    <t>Word Break II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-break-ii/</t>
+  </si>
+  <si>
+    <t>Linked List Cycle</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle/</t>
+  </si>
+  <si>
+    <t>Linked List Cycle II</t>
+  </si>
+  <si>
+    <t>2 pointers not yet</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle-ii/</t>
+  </si>
+  <si>
+    <t>Reorder List</t>
+  </si>
+  <si>
+    <t>recursive not yet</t>
+  </si>
+  <si>
+    <t>Binary Tree Preorder Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-preorder-traversal/</t>
+  </si>
+  <si>
+    <t>keeps topology$$</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-postorder-traversal/</t>
+  </si>
+  <si>
+    <t>Binary Tree Postorder Traversal</t>
+  </si>
+  <si>
+    <t>LRU Cache</t>
+  </si>
+  <si>
+    <t>design</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lru-cache/</t>
+  </si>
+  <si>
+    <t>Insertion Sort List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insertion-sort-list/</t>
+  </si>
+  <si>
+    <t>Sort List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-list/</t>
+  </si>
+  <si>
+    <t>O(1) space not yet</t>
+  </si>
+  <si>
+    <t>Max Points on a Line</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/max-points-on-a-line/</t>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>Evaluate Reverse Polish Notation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/evaluate-reverse-polish-notation/</t>
+  </si>
+  <si>
+    <t>Reverse Words in a String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-words-in-a-string/</t>
+  </si>
+  <si>
+    <t>just think about follow up</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-product-subarray/</t>
+  </si>
+  <si>
+    <t>Maximum Product Subarray</t>
+  </si>
+  <si>
+    <t>Sliding Window Maximum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sliding-window-maximum/</t>
+  </si>
+  <si>
+    <t>dp&amp;deque$$$</t>
+  </si>
+  <si>
+    <t>Boundary of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/boundary-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>Critical Connections in a Network</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/critical-connections-in-a-network/</t>
+  </si>
+  <si>
+    <t>Remove Invalid Parentheses</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-invalid-parentheses/</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array II</t>
+  </si>
+  <si>
+    <t>compare to 81 next time</t>
+  </si>
+  <si>
+    <t>compare to 33 next time</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-minimum-in-rotated-sorted-array-ii/</t>
+  </si>
+  <si>
+    <t>Min Stack</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/min-stack/</t>
+  </si>
+  <si>
+    <t>Binary Tree Upside Down</t>
+  </si>
+  <si>
+    <t>trash</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-upside-down/</t>
+  </si>
+  <si>
+    <t>Read N Characters Given Read4</t>
+  </si>
+  <si>
+    <t>try to make code cleaner</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/read-n-characters-given-read4/</t>
+  </si>
+  <si>
+    <t>Read N Characters Given Read4 II - Call multiple times</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/read-n-characters-given-read4-ii-call-multiple-times/</t>
+  </si>
+  <si>
+    <t>Longest Substring with At Most Two Distinct Characters</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-substring-with-at-most-two-distinct-characters/</t>
+  </si>
+  <si>
+    <t>just do 340</t>
+  </si>
+  <si>
+    <t>Intersection of Two Linked Lists</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/intersection-of-two-linked-lists/</t>
+  </si>
+  <si>
+    <t>One Edit Distance</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/one-edit-distance/submissions/</t>
+  </si>
+  <si>
+    <t>not yet, not enough test case</t>
+  </si>
+  <si>
+    <t>Find Peak Element</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-peak-element/</t>
+  </si>
+  <si>
+    <t>Missing Ranges</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/missing-ranges/</t>
+  </si>
+  <si>
+    <t>Maximum Gap</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-gap/</t>
+  </si>
+  <si>
+    <t>Compare Version Numbers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/compare-version-numbers/</t>
+  </si>
+  <si>
+    <t>Fraction to Recurring Decimal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/fraction-to-recurring-decimal/</t>
+  </si>
+  <si>
+    <t>how to prove 2 pointers will not let us miss numbers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/two-sum-ii-input-array-is-sorted/submissions/</t>
+  </si>
+  <si>
+    <t>Two Sum II - Input array is sorted</t>
+  </si>
+  <si>
+    <t>Excel Sheet Column Title</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/excel-sheet-column-title/</t>
+  </si>
+  <si>
+    <t>watch out edge case</t>
+  </si>
+  <si>
+    <t>Majority Element</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/majority-element/</t>
+  </si>
+  <si>
+    <t>Two Sum III</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/two-sum-iii-data-structure-design/</t>
+  </si>
+  <si>
+    <t>consider the trade-off</t>
+  </si>
+  <si>
+    <t>Excel Sheet Column Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/excel-sheet-column-number/</t>
+  </si>
+  <si>
+    <t>Factorial Trailing Zeroes</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/factorial-trailing-zeroes/</t>
+  </si>
+  <si>
+    <t>Binary Search Tree Iterator</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-search-tree-iterator/</t>
+  </si>
+  <si>
+    <t>Largest Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/largest-number/</t>
+  </si>
+  <si>
+    <t>Reverse Words in a String II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-words-in-a-string-ii/</t>
+  </si>
+  <si>
+    <t>not yet$$</t>
+  </si>
+  <si>
+    <t>Dungeon Game</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/dungeon-game/</t>
+  </si>
+  <si>
+    <t>Repeated DNA Sequences</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/repeated-dna-sequences/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-iv/</t>
+  </si>
+  <si>
+    <t>Rotate Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotate-array/</t>
+  </si>
+  <si>
+    <t>O(1) space</t>
+  </si>
+  <si>
+    <t>Reverse Bits</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-bits/</t>
+  </si>
+  <si>
+    <t>see solution in md</t>
+  </si>
+  <si>
+    <t>Number of 1 Bits</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-1-bits/</t>
+  </si>
+  <si>
+    <t>House Robber</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/house-robber/</t>
+  </si>
+  <si>
+    <t>Binary Tree Right Side View</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-right-side-view/</t>
+  </si>
+  <si>
+    <t>Number of Islands</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-islands/</t>
   </si>
 </sst>
 </file>
@@ -926,7 +1559,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
@@ -935,6 +1568,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1250,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF1DFDB-3B0E-374C-823F-F15857147895}">
-  <dimension ref="A1:I106"/>
+  <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="158" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="158" workbookViewId="0">
+      <selection activeCell="I195" sqref="I195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2929,6 +3563,1385 @@
       </c>
       <c r="I106" s="2" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>101</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>102</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>103</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>104</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B111">
+        <v>105</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>106</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B113">
+        <v>107</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>108</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="4">
+        <v>44355</v>
+      </c>
+      <c r="B115">
+        <v>109</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B116">
+        <v>110</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>111</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>112</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>113</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B120">
+        <v>114</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>115</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" s="4">
+        <v>44356</v>
+      </c>
+      <c r="B122">
+        <v>116</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I122" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B123">
+        <v>117</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="I123" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B124">
+        <v>118</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I124" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B125">
+        <v>119</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I125" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B126">
+        <v>120</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="I126" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B127">
+        <v>121</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I127" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B128">
+        <v>122</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I128" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" s="4">
+        <v>44357</v>
+      </c>
+      <c r="B129">
+        <v>123</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I129" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B130">
+        <v>124</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I130" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>125</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I131" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B132">
+        <v>126</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I132" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B133">
+        <v>127</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I133" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B134">
+        <v>128</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B135">
+        <v>129</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I135" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A136" s="4">
+        <v>44358</v>
+      </c>
+      <c r="B136">
+        <v>130</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="I136" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B137">
+        <v>131</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I137" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B138">
+        <v>132</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I138" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B139">
+        <v>133</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="I139" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B140">
+        <v>134</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="I140" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B141">
+        <v>135</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I141" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B142">
+        <v>136</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="I142" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A143" s="4">
+        <v>44359</v>
+      </c>
+      <c r="B143">
+        <v>137</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I143" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B144">
+        <v>138</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="I144" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B145">
+        <v>139</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I145" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A146" s="4">
+        <v>44360</v>
+      </c>
+      <c r="B146">
+        <v>140</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I146" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B147">
+        <v>141</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I147" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B148">
+        <v>142</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="I148" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A149" s="4">
+        <v>44361</v>
+      </c>
+      <c r="B149">
+        <v>143</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="I149" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B150">
+        <v>144</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I150" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B151">
+        <v>145</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="I151" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B152">
+        <v>146</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I152" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B153">
+        <v>147</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I153" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B154">
+        <v>148</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="I154" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B155">
+        <v>149</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="I155" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A156" s="4">
+        <v>44362</v>
+      </c>
+      <c r="B156">
+        <v>150</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I156" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B157">
+        <v>151</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="I157" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B158">
+        <v>152</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="I158" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A159" s="4">
+        <v>44363</v>
+      </c>
+      <c r="B159">
+        <v>239</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="I159" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B160">
+        <v>545</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I160" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B161">
+        <v>1192</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="I161" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B162">
+        <v>301</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="I162" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B163">
+        <v>153</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="I163" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B164">
+        <v>154</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="I164" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B165">
+        <v>155</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I165" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A166" s="4">
+        <v>44364</v>
+      </c>
+      <c r="B166">
+        <v>156</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="I166" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B167">
+        <v>157</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="I167" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B168">
+        <v>158</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I168" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B169">
+        <v>159</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="I169" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B170">
+        <v>160</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I170" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B171">
+        <v>161</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I171" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B172">
+        <v>162</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I172" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A173" s="4">
+        <v>44365</v>
+      </c>
+      <c r="B173">
+        <v>163</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I173" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B174">
+        <v>164</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I174" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B175">
+        <v>165</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I175" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B176">
+        <v>167</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="I176" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B177">
+        <v>168</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="I177" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B178">
+        <v>169</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I178" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A179" s="4">
+        <v>44366</v>
+      </c>
+      <c r="B179">
+        <v>166</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="I179" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B180">
+        <v>170</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="I180" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B181">
+        <v>171</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I181" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B182">
+        <v>172</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I182" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B183">
+        <v>173</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I183" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B184">
+        <v>179</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I184" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B185">
+        <v>186</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I185" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A186" s="4">
+        <v>44367</v>
+      </c>
+      <c r="B186" s="8">
+        <v>174</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="I186" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B187" s="8">
+        <v>187</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I187" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B188" s="8">
+        <v>188</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="I188" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B189" s="8">
+        <v>189</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="I189" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B190" s="8">
+        <v>190</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="I190" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A191" s="4">
+        <v>44368</v>
+      </c>
+      <c r="B191" s="8">
+        <v>191</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="I191" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B192" s="8">
+        <v>198</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I192" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="193" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B193" s="8">
+        <v>199</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I193" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="194" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B194" s="8">
+        <v>200</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I194" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -3036,6 +5049,94 @@
     <hyperlink ref="I104" r:id="rId101" xr:uid="{A39FF3BB-7F7F-CC48-AEFC-34269EEADB06}"/>
     <hyperlink ref="I105" r:id="rId102" xr:uid="{D2C587ED-991A-F240-A45D-61AF67D9BA87}"/>
     <hyperlink ref="I106" r:id="rId103" xr:uid="{628B66FB-BE95-3E48-B2D8-A20797DF7D0F}"/>
+    <hyperlink ref="I107" r:id="rId104" xr:uid="{41AF08F4-5FC2-3A4D-BD97-3D259DED453E}"/>
+    <hyperlink ref="I108" r:id="rId105" xr:uid="{CCF11DBB-8449-0D42-8761-688A4851D487}"/>
+    <hyperlink ref="I109" r:id="rId106" xr:uid="{D9A45B0C-2540-A24D-8763-EBFEAD93F6DD}"/>
+    <hyperlink ref="I110" r:id="rId107" xr:uid="{06306012-2F5F-A146-BC3C-47220DA5CB46}"/>
+    <hyperlink ref="I111" r:id="rId108" xr:uid="{1B5A76B8-EB89-C342-9196-DA3D490CF8D3}"/>
+    <hyperlink ref="I112" r:id="rId109" xr:uid="{46B12A61-60F1-1E49-A1B6-9E77713EB37A}"/>
+    <hyperlink ref="I113" r:id="rId110" xr:uid="{F5799FA1-1163-AB44-805E-294E06500A24}"/>
+    <hyperlink ref="I114" r:id="rId111" xr:uid="{A39FFCA4-8C2A-9B4D-B11D-6B755EC5B407}"/>
+    <hyperlink ref="I115" r:id="rId112" xr:uid="{6D3CE32F-3516-624F-8B90-3CDBA8D2CAF8}"/>
+    <hyperlink ref="I116" r:id="rId113" xr:uid="{443F4ACF-9C6F-2946-A971-AF1D0D574BE0}"/>
+    <hyperlink ref="I117" r:id="rId114" xr:uid="{27D5BEB1-4F74-3445-AC97-B84BACCD5596}"/>
+    <hyperlink ref="I118" r:id="rId115" xr:uid="{105E4580-2988-3248-AF97-6D932619C4E5}"/>
+    <hyperlink ref="I119" r:id="rId116" xr:uid="{7F4C42F5-C6D8-8B4B-9515-259E9D4155E9}"/>
+    <hyperlink ref="I120" r:id="rId117" xr:uid="{53308524-9B19-8D4F-9BB4-C37C1C777237}"/>
+    <hyperlink ref="I121" r:id="rId118" xr:uid="{61966E3C-F2AD-504F-B647-41D8E6D297B2}"/>
+    <hyperlink ref="I122" r:id="rId119" xr:uid="{D93C1040-7010-9241-AD9B-E9822E599E47}"/>
+    <hyperlink ref="I123" r:id="rId120" xr:uid="{36739098-2666-4048-B484-A5F8D25164CC}"/>
+    <hyperlink ref="I124" r:id="rId121" xr:uid="{64BEC072-FA68-1A4E-A9BE-67D405F29B19}"/>
+    <hyperlink ref="I125" r:id="rId122" xr:uid="{10FD978F-8089-9D4F-BC00-43A4EF5DE3A8}"/>
+    <hyperlink ref="I126" r:id="rId123" xr:uid="{E25A6AA0-F741-3D4B-AF69-58B151795C36}"/>
+    <hyperlink ref="I127" r:id="rId124" xr:uid="{35BF4477-CFDE-B846-B9DC-BB543456555F}"/>
+    <hyperlink ref="I128" r:id="rId125" xr:uid="{7974E2C2-C59A-5547-9AE4-A5AC9503F29C}"/>
+    <hyperlink ref="I129" r:id="rId126" xr:uid="{D98FCA19-7F00-3345-8240-49BFC5675963}"/>
+    <hyperlink ref="I130" r:id="rId127" xr:uid="{6FF01563-B736-AC4A-B975-51946858B4CA}"/>
+    <hyperlink ref="I131" r:id="rId128" xr:uid="{F7A56E8A-8E47-3A48-9C05-B6B6B1E5F267}"/>
+    <hyperlink ref="I132" r:id="rId129" xr:uid="{AD4E2386-DE12-1141-83BD-591ACF88E4BA}"/>
+    <hyperlink ref="I133" r:id="rId130" xr:uid="{551C028F-260C-FD4F-9B0D-35087330B72B}"/>
+    <hyperlink ref="I135" r:id="rId131" xr:uid="{762326B5-CF9F-FE4E-85E3-5961F0CA26AE}"/>
+    <hyperlink ref="I134" r:id="rId132" xr:uid="{E7E8177B-7577-E04D-804C-034F06DA3944}"/>
+    <hyperlink ref="I136" r:id="rId133" xr:uid="{94A5895C-012F-A24E-948F-CB86A572189E}"/>
+    <hyperlink ref="I137" r:id="rId134" xr:uid="{4516D859-9C6E-B441-8592-768FEB696CF8}"/>
+    <hyperlink ref="I138" r:id="rId135" xr:uid="{A92C2D55-14E1-3A4D-B144-6D757FCEB873}"/>
+    <hyperlink ref="I139" r:id="rId136" xr:uid="{D278F883-4EC5-384A-BB05-FB38312A1CF3}"/>
+    <hyperlink ref="I140" r:id="rId137" xr:uid="{914008AA-5A0B-7C41-B523-31641FED7006}"/>
+    <hyperlink ref="I142" r:id="rId138" xr:uid="{B8304E8B-6277-1C4E-BC9C-FBC314476511}"/>
+    <hyperlink ref="I141" r:id="rId139" xr:uid="{1806CFEC-4F5D-5B48-BB80-9E56D5B4DA33}"/>
+    <hyperlink ref="I143" r:id="rId140" xr:uid="{2D97E1A2-CCB1-2C42-91EF-CDB933CD9390}"/>
+    <hyperlink ref="I144" r:id="rId141" xr:uid="{E3216C64-B97B-8F46-9F60-F363D14A3695}"/>
+    <hyperlink ref="I145" r:id="rId142" xr:uid="{894CA520-57C0-234D-98E4-6D35607114EC}"/>
+    <hyperlink ref="I146" r:id="rId143" xr:uid="{E34C0AF5-B0B6-3444-8BD3-530DBCA463C1}"/>
+    <hyperlink ref="I147" r:id="rId144" xr:uid="{E9996E13-B533-2642-8982-D80F5AD6E011}"/>
+    <hyperlink ref="I148" r:id="rId145" xr:uid="{BD8FA801-52D3-B44D-BEF5-EB33E5A49F52}"/>
+    <hyperlink ref="I149" r:id="rId146" xr:uid="{4008538E-6963-8045-8CA1-9DF366BB1127}"/>
+    <hyperlink ref="I150" r:id="rId147" xr:uid="{CFFEC608-D996-0A4F-AF1B-0D27C4918C03}"/>
+    <hyperlink ref="I151" r:id="rId148" xr:uid="{BC9E92CD-4D69-5D43-A307-4C0C639A6721}"/>
+    <hyperlink ref="I152" r:id="rId149" xr:uid="{2870F828-9967-1C49-B045-02CF7F9939FB}"/>
+    <hyperlink ref="I153" r:id="rId150" xr:uid="{03C78FBA-ACF0-864F-BAC0-F0E391708D5E}"/>
+    <hyperlink ref="I154" r:id="rId151" xr:uid="{4C20201F-FC6E-4149-8049-F81C8026DBFF}"/>
+    <hyperlink ref="I155" r:id="rId152" xr:uid="{3B73680B-7194-F84A-B996-62D39862FBC1}"/>
+    <hyperlink ref="I156" r:id="rId153" xr:uid="{5F6216EF-433D-9445-88C0-D379CE0CFB43}"/>
+    <hyperlink ref="I157" r:id="rId154" xr:uid="{502F4DC0-206A-6C40-8C13-8F9302D197F1}"/>
+    <hyperlink ref="I158" r:id="rId155" xr:uid="{F127A0AA-8028-8040-A62C-F4A5634EAA82}"/>
+    <hyperlink ref="I159" r:id="rId156" xr:uid="{4E2FCCC0-F49D-994C-8C96-A28B4DBCD228}"/>
+    <hyperlink ref="I160" r:id="rId157" xr:uid="{0EEE29C3-A688-DD45-988B-4051F37FB078}"/>
+    <hyperlink ref="I161" r:id="rId158" xr:uid="{28EC712D-23C1-0043-A716-76E6A2A5399F}"/>
+    <hyperlink ref="I162" r:id="rId159" xr:uid="{AA74063E-3C12-1A41-83F1-0510046F6140}"/>
+    <hyperlink ref="I163" r:id="rId160" xr:uid="{D0CC5E9C-66D6-C442-8483-9567889D61D1}"/>
+    <hyperlink ref="I164" r:id="rId161" xr:uid="{B35A8832-484B-444D-8670-423EF98C0ADA}"/>
+    <hyperlink ref="I165" r:id="rId162" xr:uid="{8421A30F-60D6-E640-8AD1-CB221A39BEE7}"/>
+    <hyperlink ref="I166" r:id="rId163" xr:uid="{C285FBCF-8C13-C447-8BAD-D4C24059B524}"/>
+    <hyperlink ref="I167" r:id="rId164" xr:uid="{1B11DE61-734A-E949-913E-C59D7A0BC2EA}"/>
+    <hyperlink ref="I168" r:id="rId165" xr:uid="{491004AB-D567-4A47-9BC1-E34CB859803E}"/>
+    <hyperlink ref="I169" r:id="rId166" xr:uid="{61EDC545-9F93-DE4D-BED3-1E3517B05C70}"/>
+    <hyperlink ref="I170" r:id="rId167" xr:uid="{3A60D012-B475-EF49-8FA8-DCA05DE1D4E5}"/>
+    <hyperlink ref="I171" r:id="rId168" xr:uid="{5CFCE4CA-7D45-4845-BB94-021F9E6F5BA9}"/>
+    <hyperlink ref="I172" r:id="rId169" xr:uid="{E862D60B-37DD-394A-84F1-6FDB12E02835}"/>
+    <hyperlink ref="I173" r:id="rId170" xr:uid="{DE89E0D9-504B-7649-9FAF-A492C1709276}"/>
+    <hyperlink ref="I174" r:id="rId171" xr:uid="{D7476C6D-A3B0-1244-BC81-DFECB5FF6DD6}"/>
+    <hyperlink ref="I175" r:id="rId172" xr:uid="{0C1F9FE4-8524-9147-B739-F3960A42D626}"/>
+    <hyperlink ref="I179" r:id="rId173" xr:uid="{98C91998-3195-EA42-81EC-3E11B7DC474C}"/>
+    <hyperlink ref="I176" r:id="rId174" xr:uid="{18D6E95B-6934-8D49-A37E-F69A3E7F3547}"/>
+    <hyperlink ref="I177" r:id="rId175" xr:uid="{A7A6E0E9-FAFE-7B40-9670-9258F3222223}"/>
+    <hyperlink ref="I178" r:id="rId176" xr:uid="{64D27079-3B22-0C4E-BA15-007702A6B3C9}"/>
+    <hyperlink ref="I180" r:id="rId177" xr:uid="{2A55F561-14C5-CA43-BC2A-85B79C5E0BA2}"/>
+    <hyperlink ref="I181" r:id="rId178" xr:uid="{2BBEB7C4-6E2A-0349-A5A2-505FC600CB2D}"/>
+    <hyperlink ref="I182" r:id="rId179" xr:uid="{8A734B3B-3B03-444C-A34A-F9E28EC9AF05}"/>
+    <hyperlink ref="I183" r:id="rId180" xr:uid="{014F2C7F-1E89-924C-843E-12E09D9236B2}"/>
+    <hyperlink ref="I184" r:id="rId181" xr:uid="{7D701299-0803-D44A-B77C-E8D0FFB2A97A}"/>
+    <hyperlink ref="I185" r:id="rId182" xr:uid="{AA7CF1AE-AD87-C34D-9916-35410B0EA4C7}"/>
+    <hyperlink ref="I186" r:id="rId183" xr:uid="{20EC7595-5B2A-2346-9196-D29CC7882C2B}"/>
+    <hyperlink ref="I187" r:id="rId184" xr:uid="{51D820A2-F115-0949-A0F8-D6B96B874F3D}"/>
+    <hyperlink ref="I188" r:id="rId185" xr:uid="{E029140A-335F-1B45-9F18-C31BFF74D4C6}"/>
+    <hyperlink ref="I189" r:id="rId186" xr:uid="{5B7E6F79-BBB1-2B4C-B0DA-5123009A8A2A}"/>
+    <hyperlink ref="I190" r:id="rId187" xr:uid="{9FD5FFDF-0689-2741-9773-E523298B7814}"/>
+    <hyperlink ref="I191" r:id="rId188" xr:uid="{E95C1453-4C67-BD4E-BDA2-E81BC92F2FDC}"/>
+    <hyperlink ref="I192" r:id="rId189" xr:uid="{8603DC82-F3DC-3641-A4E6-98169C677C05}"/>
+    <hyperlink ref="I193" r:id="rId190" xr:uid="{8A791F43-FADA-D143-9127-2398A77CAB79}"/>
+    <hyperlink ref="I194" r:id="rId191" xr:uid="{9462EB8A-80F6-4241-B7A2-482752EEC499}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>